<commit_message>
Random shizzle for the spreadsheet
Doing stats from one recent game in the EU LCS
</commit_message>
<xml_diff>
--- a/Spreadsheet.xlsx
+++ b/Spreadsheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0AD6D8F-CDE4-455B-A3A1-93A9099F4DB9}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA52748-2196-4A52-9619-47F0DCFE5660}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,18 +20,81 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>Hej</t>
-  </si>
-  <si>
-    <t>sda</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>sad</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>League</t>
+  </si>
+  <si>
+    <t>Blue Team</t>
+  </si>
+  <si>
+    <t>Red Team</t>
+  </si>
+  <si>
+    <t>FTRT</t>
+  </si>
+  <si>
+    <t>FTBT</t>
+  </si>
+  <si>
+    <t>FTR</t>
+  </si>
+  <si>
+    <t>EU LCS</t>
+  </si>
+  <si>
+    <t>Splyce</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>GBT</t>
+  </si>
+  <si>
+    <t>GRT</t>
+  </si>
+  <si>
+    <t>KBT</t>
+  </si>
+  <si>
+    <t>KRT</t>
+  </si>
+  <si>
+    <t>WBT</t>
+  </si>
+  <si>
+    <t>WRT</t>
+  </si>
+  <si>
+    <t>TDBT</t>
+  </si>
+  <si>
+    <t>TDRT</t>
+  </si>
+  <si>
+    <t>FBBT</t>
+  </si>
+  <si>
+    <t>FBRT</t>
+  </si>
+  <si>
+    <t>CWBT</t>
+  </si>
+  <si>
+    <t>CWRT</t>
+  </si>
+  <si>
+    <t>RBT</t>
+  </si>
+  <si>
+    <t>RRT</t>
   </si>
 </sst>
 </file>
@@ -67,8 +130,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -349,40 +413,142 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:U2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="U1" sqref="U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" t="s">
+        <v>17</v>
+      </c>
+      <c r="O1" t="s">
+        <v>18</v>
+      </c>
+      <c r="P1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" t="s">
+        <v>21</v>
+      </c>
+      <c r="S1" t="s">
+        <v>22</v>
+      </c>
+      <c r="T1" t="s">
+        <v>23</v>
+      </c>
+      <c r="U1" t="s">
+        <v>24</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1">
+        <v>43176</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>2</v>
+      <c r="G2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2">
+        <v>52000</v>
+      </c>
+      <c r="I2">
+        <v>64800</v>
+      </c>
+      <c r="J2">
+        <v>6</v>
+      </c>
+      <c r="K2">
+        <v>15</v>
+      </c>
+      <c r="L2">
+        <v>125</v>
+      </c>
+      <c r="M2">
+        <v>142</v>
+      </c>
+      <c r="N2">
+        <v>45400</v>
+      </c>
+      <c r="O2">
+        <v>64100</v>
+      </c>
+      <c r="P2">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>41</v>
+      </c>
+      <c r="S2">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>